<commit_message>
Completed EDA for 184
</commit_message>
<xml_diff>
--- a/CH-184 Table Transformation.xlsx
+++ b/CH-184 Table Transformation.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{34244A51-178A-4301-A4BD-A424CA71B03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F4249-6519-430D-BD95-C82709E8BAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="1" r:id="rId1"/>
+    <sheet name="EDA" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,8 +36,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
   <si>
     <t>Result</t>
   </si>
@@ -494,6 +517,128 @@
         <a:xfrm>
           <a:off x="3076575" y="2381250"/>
           <a:ext cx="2676525" cy="1647825"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartAlternateProcess">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1800" b="1">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Challenge 184:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1800" b="1" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FFFF00"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Table Transformation!</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-AU" sz="1100" b="1" baseline="0">
+            <a:solidFill>
+              <a:srgbClr val="FFFF00"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1600" b="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+            </a:rPr>
+            <a:t>Transform the question structure into the result structure.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E3FA79B-739F-4C98-B747-5C5DD197A136}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2407920" y="2221230"/>
+          <a:ext cx="2676525" cy="1518285"/>
         </a:xfrm>
         <a:prstGeom prst="flowChartAlternateProcess">
           <a:avLst/>
@@ -850,12 +995,39 @@
 </a:theme>
 </file>
 
+<file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
+<wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
+  <wetp:taskpane dockstate="right" visibility="0" width="536" row="8">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+</wetp:taskpanes>
+</file>
+
+<file path=xl/webextensions/webextension1.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{9B857F6D-8890-4314-9CEC-6D5834745034}">
+  <we:reference id="wa200003696" version="1.3.0.0" store="en-US" storeType="OMEX"/>
+  <we:alternateReferences>
+    <we:reference id="wa200003696" version="1.3.0.0" store="" storeType="OMEX"/>
+  </we:alternateReferences>
+  <we:properties/>
+  <we:bindings/>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+  <we:extLst>
+    <a:ext xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uri="{7C84B067-C214-45C3-A712-C9D94CD141B2}">
+      <we:customFunctionIdList>
+        <we:customFunctionIds>_xldudf_LABS_GENERATIVEAI</we:customFunctionIds>
+      </we:customFunctionIdList>
+    </a:ext>
+  </we:extLst>
+</we:webextension>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1078,6 +1250,738 @@
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540FF978-6B88-4122-B777-AFDA0F3A2BEC}">
+  <dimension ref="B1:Q38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.8984375" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" style="5" customWidth="1"/>
+    <col min="4" max="4" width="10.5" style="9" customWidth="1"/>
+    <col min="5" max="7" width="10.5" style="5" customWidth="1"/>
+    <col min="11" max="11" width="10.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="4"/>
+      <c r="E1" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="L1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="2:12" s="2" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="C2" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="4"/>
+      <c r="E2" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C3" s="23">
+        <v>45493</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="13">
+        <v>45493</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3" s="15">
+        <v>10</v>
+      </c>
+      <c r="I3" s="1" t="b">
+        <f>ISNUMBER(G3)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C4" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5"/>
+      <c r="E4" s="11">
+        <v>45509</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="7">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="24">
+        <v>45509</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="11">
+        <v>45509</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G5" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="11">
+        <v>45509</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C7" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="5"/>
+      <c r="E7" s="27">
+        <v>45517</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="16">
+        <v>45553</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="G8" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="26">
+        <v>45517</v>
+      </c>
+      <c r="D9" s="5"/>
+      <c r="E9" s="16">
+        <v>45553</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="16">
+        <v>45553</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="25">
+        <v>45553</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="11">
+        <v>45566</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C12" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" s="12">
+        <v>45566</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C13" s="25" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C15" s="24">
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="C16" s="24" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C17" s="24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C24" s="23" cm="1">
+        <f t="array" ref="C24:C38">_xlfn.SCAN(
+"",
+C3:C17+0,
+_xlfn.LAMBDA(_xlpm.a,_xlpm.v,
+IF(ISNUMBER(_xlpm.v),_xlpm.v,_xlfn.TAKE(_xlpm.a,-1))
+)
+)</f>
+        <v>45493</v>
+      </c>
+      <c r="D24" s="23" cm="1">
+        <f t="array" ref="D24:D38">IF(ISTEXT(C3:C17),C3:C17,C3:C17+0)</f>
+        <v>45493</v>
+      </c>
+      <c r="E24" s="5" t="str" cm="1">
+        <f t="array" ref="E24">_xlfn.TEXTSPLIT(D24,",")</f>
+        <v>45493</v>
+      </c>
+      <c r="G24" s="13" cm="1">
+        <f t="array" ref="G24:I33">_xlfn._xlws.FILTER(_xlfn.HSTACK(_xlfn.ANCHORARRAY(C24),E24:F38),1-ISBLANK(F24:F38))</f>
+        <v>45493</v>
+      </c>
+      <c r="H24" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="I24" s="15" t="str">
+        <v xml:space="preserve"> 10</v>
+      </c>
+      <c r="K24" s="13" cm="1">
+        <f t="array" ref="K24:L33">G24:H33</f>
+        <v>45493</v>
+      </c>
+      <c r="L24" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="M24" s="15" cm="1">
+        <f t="array" ref="M24:M33">I24:I33+0</f>
+        <v>10</v>
+      </c>
+      <c r="O24" t="b" cm="1">
+        <f t="array" ref="O24:Q33">K24:M33=E3:G12</f>
+        <v>1</v>
+      </c>
+      <c r="P24" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="23">
+        <v>45493</v>
+      </c>
+      <c r="D25" s="23" t="str">
+        <v>A, 10</v>
+      </c>
+      <c r="E25" s="5" t="str" cm="1">
+        <f t="array" ref="E25:F25">_xlfn.TEXTSPLIT(D25,",")</f>
+        <v>A</v>
+      </c>
+      <c r="F25" s="5" t="str">
+        <v xml:space="preserve"> 10</v>
+      </c>
+      <c r="G25" s="11">
+        <v>45509</v>
+      </c>
+      <c r="H25" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="I25" s="7" t="str">
+        <v xml:space="preserve"> 8</v>
+      </c>
+      <c r="K25" s="11">
+        <v>45509</v>
+      </c>
+      <c r="L25" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="M25" s="7">
+        <v>8</v>
+      </c>
+      <c r="O25" t="b">
+        <v>1</v>
+      </c>
+      <c r="P25" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C26" s="23">
+        <v>45509</v>
+      </c>
+      <c r="D26" s="24">
+        <v>45509</v>
+      </c>
+      <c r="E26" s="5" t="str" cm="1">
+        <f t="array" ref="E26">_xlfn.TEXTSPLIT(D26,",")</f>
+        <v>45509</v>
+      </c>
+      <c r="G26" s="11">
+        <v>45509</v>
+      </c>
+      <c r="H26" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="I26" s="7" t="str">
+        <v xml:space="preserve"> 2</v>
+      </c>
+      <c r="K26" s="11">
+        <v>45509</v>
+      </c>
+      <c r="L26" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="M26" s="7">
+        <v>2</v>
+      </c>
+      <c r="O26" t="b">
+        <v>1</v>
+      </c>
+      <c r="P26" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C27" s="23">
+        <v>45509</v>
+      </c>
+      <c r="D27" s="24" t="str">
+        <v>C, 8</v>
+      </c>
+      <c r="E27" s="5" t="str" cm="1">
+        <f t="array" ref="E27:F27">_xlfn.TEXTSPLIT(D27,",")</f>
+        <v>C</v>
+      </c>
+      <c r="F27" s="5" t="str">
+        <v xml:space="preserve"> 8</v>
+      </c>
+      <c r="G27" s="11">
+        <v>45509</v>
+      </c>
+      <c r="H27" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="I27" s="7" t="str">
+        <v xml:space="preserve"> 2</v>
+      </c>
+      <c r="K27" s="11">
+        <v>45509</v>
+      </c>
+      <c r="L27" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="M27" s="7">
+        <v>2</v>
+      </c>
+      <c r="O27" t="b">
+        <v>1</v>
+      </c>
+      <c r="P27" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C28" s="23">
+        <v>45509</v>
+      </c>
+      <c r="D28" s="24" t="str">
+        <v>B, 2</v>
+      </c>
+      <c r="E28" s="5" t="str" cm="1">
+        <f t="array" ref="E28:F28">_xlfn.TEXTSPLIT(D28,",")</f>
+        <v>B</v>
+      </c>
+      <c r="F28" s="5" t="str">
+        <v xml:space="preserve"> 2</v>
+      </c>
+      <c r="G28" s="27">
+        <v>45517</v>
+      </c>
+      <c r="H28" s="28" t="str">
+        <v>B</v>
+      </c>
+      <c r="I28" s="29" t="str">
+        <v xml:space="preserve"> 1</v>
+      </c>
+      <c r="K28" s="27">
+        <v>45517</v>
+      </c>
+      <c r="L28" s="28" t="str">
+        <v>B</v>
+      </c>
+      <c r="M28" s="29">
+        <v>1</v>
+      </c>
+      <c r="O28" t="b">
+        <v>1</v>
+      </c>
+      <c r="P28" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C29" s="23">
+        <v>45509</v>
+      </c>
+      <c r="D29" s="24" t="str">
+        <v>A, 2</v>
+      </c>
+      <c r="E29" s="5" t="str" cm="1">
+        <f t="array" ref="E29:F29">_xlfn.TEXTSPLIT(D29,",")</f>
+        <v>A</v>
+      </c>
+      <c r="F29" s="5" t="str">
+        <v xml:space="preserve"> 2</v>
+      </c>
+      <c r="G29" s="16">
+        <v>45553</v>
+      </c>
+      <c r="H29" s="17" t="str">
+        <v>A</v>
+      </c>
+      <c r="I29" s="18" t="str">
+        <v xml:space="preserve"> 5</v>
+      </c>
+      <c r="K29" s="16">
+        <v>45553</v>
+      </c>
+      <c r="L29" s="17" t="str">
+        <v>A</v>
+      </c>
+      <c r="M29" s="18">
+        <v>5</v>
+      </c>
+      <c r="O29" t="b">
+        <v>1</v>
+      </c>
+      <c r="P29" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C30" s="23">
+        <v>45517</v>
+      </c>
+      <c r="D30" s="26">
+        <v>45517</v>
+      </c>
+      <c r="E30" s="5" t="str" cm="1">
+        <f t="array" ref="E30">_xlfn.TEXTSPLIT(D30,",")</f>
+        <v>45517</v>
+      </c>
+      <c r="G30" s="16">
+        <v>45553</v>
+      </c>
+      <c r="H30" s="17" t="str">
+        <v>B</v>
+      </c>
+      <c r="I30" s="18" t="str">
+        <v xml:space="preserve"> 4</v>
+      </c>
+      <c r="K30" s="16">
+        <v>45553</v>
+      </c>
+      <c r="L30" s="17" t="str">
+        <v>B</v>
+      </c>
+      <c r="M30" s="18">
+        <v>4</v>
+      </c>
+      <c r="O30" t="b">
+        <v>1</v>
+      </c>
+      <c r="P30" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C31" s="23">
+        <v>45517</v>
+      </c>
+      <c r="D31" s="26" t="str">
+        <v>B, 1</v>
+      </c>
+      <c r="E31" s="5" t="str" cm="1">
+        <f t="array" ref="E31:F31">_xlfn.TEXTSPLIT(D31,",")</f>
+        <v>B</v>
+      </c>
+      <c r="F31" s="5" t="str">
+        <v xml:space="preserve"> 1</v>
+      </c>
+      <c r="G31" s="16">
+        <v>45553</v>
+      </c>
+      <c r="H31" s="17" t="str">
+        <v>C</v>
+      </c>
+      <c r="I31" s="18" t="str">
+        <v xml:space="preserve"> 3</v>
+      </c>
+      <c r="K31" s="16">
+        <v>45553</v>
+      </c>
+      <c r="L31" s="17" t="str">
+        <v>C</v>
+      </c>
+      <c r="M31" s="18">
+        <v>3</v>
+      </c>
+      <c r="O31" t="b">
+        <v>1</v>
+      </c>
+      <c r="P31" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C32" s="23">
+        <v>45553</v>
+      </c>
+      <c r="D32" s="25">
+        <v>45553</v>
+      </c>
+      <c r="E32" s="5" t="str" cm="1">
+        <f t="array" ref="E32">_xlfn.TEXTSPLIT(D32,",")</f>
+        <v>45553</v>
+      </c>
+      <c r="G32" s="11">
+        <v>45566</v>
+      </c>
+      <c r="H32" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="I32" s="7" t="str">
+        <v xml:space="preserve"> 1</v>
+      </c>
+      <c r="K32" s="11">
+        <v>45566</v>
+      </c>
+      <c r="L32" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="M32" s="7">
+        <v>1</v>
+      </c>
+      <c r="O32" t="b">
+        <v>1</v>
+      </c>
+      <c r="P32" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C33" s="23">
+        <v>45553</v>
+      </c>
+      <c r="D33" s="25" t="str">
+        <v>A, 5</v>
+      </c>
+      <c r="E33" s="5" t="str" cm="1">
+        <f t="array" ref="E33:F33">_xlfn.TEXTSPLIT(D33,",")</f>
+        <v>A</v>
+      </c>
+      <c r="F33" s="5" t="str">
+        <v xml:space="preserve"> 5</v>
+      </c>
+      <c r="G33" s="12">
+        <v>45566</v>
+      </c>
+      <c r="H33" s="8" t="str">
+        <v>B</v>
+      </c>
+      <c r="I33" s="10" t="str">
+        <v xml:space="preserve"> 2</v>
+      </c>
+      <c r="K33" s="12">
+        <v>45566</v>
+      </c>
+      <c r="L33" s="8" t="str">
+        <v>B</v>
+      </c>
+      <c r="M33" s="10">
+        <v>2</v>
+      </c>
+      <c r="O33" t="b">
+        <v>1</v>
+      </c>
+      <c r="P33" t="b">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C34" s="23">
+        <v>45553</v>
+      </c>
+      <c r="D34" s="25" t="str">
+        <v>B, 4</v>
+      </c>
+      <c r="E34" s="5" t="str" cm="1">
+        <f t="array" ref="E34:F34">_xlfn.TEXTSPLIT(D34,",")</f>
+        <v>B</v>
+      </c>
+      <c r="F34" s="5" t="str">
+        <v xml:space="preserve"> 4</v>
+      </c>
+    </row>
+    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C35" s="23">
+        <v>45553</v>
+      </c>
+      <c r="D35" s="25" t="str">
+        <v>C, 3</v>
+      </c>
+      <c r="E35" s="5" t="str" cm="1">
+        <f t="array" ref="E35:F35">_xlfn.TEXTSPLIT(D35,",")</f>
+        <v>C</v>
+      </c>
+      <c r="F35" s="5" t="str">
+        <v xml:space="preserve"> 3</v>
+      </c>
+    </row>
+    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C36" s="23">
+        <v>45566</v>
+      </c>
+      <c r="D36" s="24">
+        <v>45566</v>
+      </c>
+      <c r="E36" s="5" t="str" cm="1">
+        <f t="array" ref="E36">_xlfn.TEXTSPLIT(D36,",")</f>
+        <v>45566</v>
+      </c>
+    </row>
+    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C37" s="23">
+        <v>45566</v>
+      </c>
+      <c r="D37" s="24" t="str">
+        <v>A, 1</v>
+      </c>
+      <c r="E37" s="5" t="str" cm="1">
+        <f t="array" ref="E37:F37">_xlfn.TEXTSPLIT(D37,",")</f>
+        <v>A</v>
+      </c>
+      <c r="F37" s="5" t="str">
+        <v xml:space="preserve"> 1</v>
+      </c>
+    </row>
+    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+      <c r="C38" s="23">
+        <v>45566</v>
+      </c>
+      <c r="D38" s="24" t="str">
+        <v>B, 2</v>
+      </c>
+      <c r="E38" s="5" t="str" cm="1">
+        <f t="array" ref="E38:F38">_xlfn.TEXTSPLIT(D38,",")</f>
+        <v>B</v>
+      </c>
+      <c r="F38" s="5" t="str">
+        <v xml:space="preserve"> 2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>

<commit_message>
Created my single function
</commit_message>
<xml_diff>
--- a/CH-184 Table Transformation.xlsx
+++ b/CH-184 Table Transformation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{999F4249-6519-430D-BD95-C82709E8BAF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2345476C-3810-4DDD-BF7A-7A2761A75DD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>Result</t>
   </si>
@@ -117,12 +117,15 @@
   <si>
     <t>https://www.linkedin.com/in/omid-motamedisedeh-74aba166/recent-activity/all/</t>
   </si>
+  <si>
+    <t>Single Function</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -164,6 +167,13 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Mono"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -203,7 +213,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -376,11 +386,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -470,8 +490,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -997,7 +1019,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="536" row="8">
+  <wetp:taskpane dockstate="right" visibility="0" width="976" row="8">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1258,10 +1280,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{540FF978-6B88-4122-B777-AFDA0F3A2BEC}">
-  <dimension ref="B1:Q38"/>
+  <dimension ref="B1:Q53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1864,7 +1886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C33" s="23">
         <v>45553</v>
       </c>
@@ -1906,7 +1928,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C34" s="23">
         <v>45553</v>
       </c>
@@ -1921,7 +1943,7 @@
         <v xml:space="preserve"> 4</v>
       </c>
     </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C35" s="23">
         <v>45553</v>
       </c>
@@ -1936,7 +1958,7 @@
         <v xml:space="preserve"> 3</v>
       </c>
     </row>
-    <row r="36" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C36" s="23">
         <v>45566</v>
       </c>
@@ -1948,7 +1970,7 @@
         <v>45566</v>
       </c>
     </row>
-    <row r="37" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C37" s="23">
         <v>45566</v>
       </c>
@@ -1963,7 +1985,7 @@
         <v xml:space="preserve"> 1</v>
       </c>
     </row>
-    <row r="38" spans="3:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
       <c r="C38" s="23">
         <v>45566</v>
       </c>
@@ -1976,6 +1998,240 @@
       </c>
       <c r="F38" s="5" t="str">
         <v xml:space="preserve"> 2</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="B40" s="31" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" ht="14.4" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C42" s="19" t="str" cm="1">
+        <f t="array" ref="C42:E52">_xlfn.LET(
+_xlpm.d, _xlfn.SCAN("", C3:C17 + 0, _xlfn.LAMBDA(_xlpm.a,_xlpm.v, IF(ISNUMBER(_xlpm.v), _xlpm.v, _xlfn.TAKE(_xlpm.a, -1)))),
+_xlpm.q, _xlfn.HSTACK(_xlpm.d,_xlfn.TEXTBEFORE(_xlfn.ANCHORARRAY(D24),","),_xlfn.TEXTAFTER(_xlfn.ANCHORARRAY(D24),",")+0),
+_xlfn.VSTACK(E2:G2,_xlfn._xlws.FILTER(_xlpm.q,NOT(ISNA(_xlfn.TAKE(_xlpm.q,,-1)))))
+)</f>
+        <v>Date</v>
+      </c>
+      <c r="D42" s="20" t="str">
+        <v>Product</v>
+      </c>
+      <c r="E42" s="21" t="str">
+        <v>Quantity</v>
+      </c>
+    </row>
+    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C43" s="13">
+        <v>45493</v>
+      </c>
+      <c r="D43" s="14" t="str">
+        <v>A</v>
+      </c>
+      <c r="E43" s="15">
+        <v>10</v>
+      </c>
+      <c r="G43" s="5" t="b" cm="1">
+        <f t="array" ref="G43:I53">_xlfn.ANCHORARRAY(C42)=E2:G12</f>
+        <v>1</v>
+      </c>
+      <c r="H43" t="b">
+        <v>1</v>
+      </c>
+      <c r="I43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C44" s="11">
+        <v>45509</v>
+      </c>
+      <c r="D44" s="6" t="str">
+        <v>C</v>
+      </c>
+      <c r="E44" s="7">
+        <v>8</v>
+      </c>
+      <c r="G44" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H44" t="b">
+        <v>1</v>
+      </c>
+      <c r="I44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C45" s="11">
+        <v>45509</v>
+      </c>
+      <c r="D45" s="6" t="str">
+        <v>B</v>
+      </c>
+      <c r="E45" s="7">
+        <v>2</v>
+      </c>
+      <c r="G45" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H45" t="b">
+        <v>1</v>
+      </c>
+      <c r="I45" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C46" s="11">
+        <v>45509</v>
+      </c>
+      <c r="D46" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="E46" s="7">
+        <v>2</v>
+      </c>
+      <c r="G46" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H46" t="b">
+        <v>1</v>
+      </c>
+      <c r="I46" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C47" s="27">
+        <v>45517</v>
+      </c>
+      <c r="D47" s="28" t="str">
+        <v>B</v>
+      </c>
+      <c r="E47" s="29">
+        <v>1</v>
+      </c>
+      <c r="G47" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H47" t="b">
+        <v>1</v>
+      </c>
+      <c r="I47" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C48" s="16">
+        <v>45553</v>
+      </c>
+      <c r="D48" s="17" t="str">
+        <v>A</v>
+      </c>
+      <c r="E48" s="18">
+        <v>5</v>
+      </c>
+      <c r="G48" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H48" t="b">
+        <v>1</v>
+      </c>
+      <c r="I48" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C49" s="16">
+        <v>45553</v>
+      </c>
+      <c r="D49" s="17" t="str">
+        <v>B</v>
+      </c>
+      <c r="E49" s="18">
+        <v>4</v>
+      </c>
+      <c r="G49" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H49" t="b">
+        <v>1</v>
+      </c>
+      <c r="I49" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C50" s="16">
+        <v>45553</v>
+      </c>
+      <c r="D50" s="17" t="str">
+        <v>C</v>
+      </c>
+      <c r="E50" s="18">
+        <v>3</v>
+      </c>
+      <c r="G50" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H50" t="b">
+        <v>1</v>
+      </c>
+      <c r="I50" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C51" s="11">
+        <v>45566</v>
+      </c>
+      <c r="D51" s="6" t="str">
+        <v>A</v>
+      </c>
+      <c r="E51" s="7">
+        <v>1</v>
+      </c>
+      <c r="G51" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H51" t="b">
+        <v>1</v>
+      </c>
+      <c r="I51" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C52" s="12">
+        <v>45566</v>
+      </c>
+      <c r="D52" s="8" t="str">
+        <v>B</v>
+      </c>
+      <c r="E52" s="10">
+        <v>2</v>
+      </c>
+      <c r="G52" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H52" t="b">
+        <v>1</v>
+      </c>
+      <c r="I52" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="G53" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H53" t="b">
+        <v>1</v>
+      </c>
+      <c r="I53" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>